<commit_message>
added cooling hose and stepper motor heatsinks
</commit_message>
<xml_diff>
--- a/Documents/SLS Machine Purchase List.xlsx
+++ b/Documents/SLS Machine Purchase List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hunter\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris_000\Documents\GitHub\AIAA-SLS\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
   <si>
     <t>Part</t>
   </si>
@@ -89,12 +89,6 @@
     <t>90473A029</t>
   </si>
   <si>
-    <t>1/4-20 low strength steel, zinc plated nuts</t>
-  </si>
-  <si>
-    <t>1/4-20 Pan Head Phillips Machine Screws, zinc plated</t>
-  </si>
-  <si>
     <t>https://www.metalsdepot.com/products/alum2.phtml?page=sheet&amp;LimAcc=%20&amp;aident=#p383</t>
   </si>
   <si>
@@ -263,9 +257,6 @@
     <t>http://www.mcmaster.com/#nylon-insert-locknuts/=113hvda</t>
   </si>
   <si>
-    <t>Zinc Yellow-Chromate Plated 1/4-20 nylon insert lock nuts</t>
-  </si>
-  <si>
     <t>1513A31</t>
   </si>
   <si>
@@ -293,7 +284,28 @@
     <t>www.mcmaster.com/#bulb-seals/=113i3mq</t>
   </si>
   <si>
-    <t>HEAT SINK</t>
+    <t>Zinc Yellow-Chromate Plated 1/4-20 nylon insert lock nuts (25pk)</t>
+  </si>
+  <si>
+    <t>1/4-20 low strength steel, zinc plated nuts (100pk)</t>
+  </si>
+  <si>
+    <t>1/4-20 Pan Head Phillips Machine Screws, zinc plated (100pk)</t>
+  </si>
+  <si>
+    <t>9mm ID high pressure air/water flex tube (10ft)</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/gp/offer-listing/B0054S6NP4/ref=dp_olp_new_mbc?ie=UTF8&amp;condition=new</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/11510</t>
+  </si>
+  <si>
+    <t>Small Heatsink (.25" x .30") for stepper motor driver Ics</t>
+  </si>
+  <si>
+    <t>PRT-11510</t>
   </si>
 </sst>
 </file>
@@ -321,18 +333,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -359,7 +365,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -641,20 +647,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="74" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.58203125" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -677,7 +683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -701,7 +707,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -718,14 +724,14 @@
         <v>2</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F27" si="0">D3*E3</f>
+        <f t="shared" ref="F3:F29" si="0">D3*E3</f>
         <v>23.58</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -746,12 +752,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>88</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>18</v>
@@ -770,9 +776,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>20</v>
@@ -788,15 +794,15 @@
         <v>2.68</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D7">
         <v>3.43</v>
@@ -809,15 +815,15 @@
         <v>3.43</v>
       </c>
       <c r="G7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8">
         <v>3.37</v>
@@ -830,15 +836,15 @@
         <v>3.37</v>
       </c>
       <c r="G8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D9">
         <v>13.43</v>
@@ -851,15 +857,15 @@
         <v>53.72</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1">
         <v>7.9</v>
@@ -872,15 +878,15 @@
         <v>15.8</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11">
         <v>6.97</v>
@@ -893,15 +899,15 @@
         <v>13.94</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D12">
         <v>3.81</v>
@@ -914,15 +920,15 @@
         <v>7.62</v>
       </c>
       <c r="G12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D13">
         <v>5.15</v>
@@ -935,15 +941,15 @@
         <v>10.3</v>
       </c>
       <c r="G13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D14">
         <v>11.03</v>
@@ -956,15 +962,15 @@
         <v>11.03</v>
       </c>
       <c r="G14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D15">
         <v>1.0900000000000001</v>
@@ -977,15 +983,15 @@
         <v>10.9</v>
       </c>
       <c r="G15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" s="4">
         <v>307609</v>
@@ -1001,12 +1007,12 @@
         <v>11.69</v>
       </c>
       <c r="G16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17" s="4">
         <v>307583</v>
@@ -1022,18 +1028,18 @@
         <v>11.69</v>
       </c>
       <c r="G17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D18">
         <v>24.52</v>
@@ -1046,18 +1052,18 @@
         <v>24.52</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D19">
         <v>170</v>
@@ -1070,18 +1076,18 @@
         <v>170</v>
       </c>
       <c r="G19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
         <v>54</v>
-      </c>
-      <c r="B20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" t="s">
-        <v>56</v>
       </c>
       <c r="D20" s="1">
         <v>6.8</v>
@@ -1094,18 +1100,18 @@
         <v>40.799999999999997</v>
       </c>
       <c r="G20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
         <v>61</v>
-      </c>
-      <c r="B21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" t="s">
-        <v>63</v>
       </c>
       <c r="D21">
         <v>0.45</v>
@@ -1118,15 +1124,15 @@
         <v>22.5</v>
       </c>
       <c r="G21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D22">
         <v>0.19</v>
@@ -1139,18 +1145,18 @@
         <v>9.5</v>
       </c>
       <c r="G22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D23">
         <v>39.97</v>
@@ -1163,15 +1169,15 @@
         <v>79.94</v>
       </c>
       <c r="G23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" t="s">
-        <v>45</v>
       </c>
       <c r="D24" s="1">
         <v>17.5</v>
@@ -1184,15 +1190,15 @@
         <v>17.5</v>
       </c>
       <c r="G24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D25">
         <v>75.84</v>
@@ -1205,15 +1211,15 @@
         <v>75.84</v>
       </c>
       <c r="G25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D26">
         <v>52</v>
@@ -1226,15 +1232,15 @@
         <v>52</v>
       </c>
       <c r="G26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D27">
         <v>39.450000000000003</v>
@@ -1247,19 +1253,52 @@
         <v>39.450000000000003</v>
       </c>
       <c r="G27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
         <v>89</v>
       </c>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>12.95</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="0"/>
+        <v>12.95</v>
+      </c>
+      <c r="G28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B29" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29">
+        <v>1.95</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
       <c r="F29" s="1">
-        <f>SUM(F2:F27)</f>
-        <v>860.12</v>
+        <f t="shared" si="0"/>
+        <v>9.75</v>
+      </c>
+      <c r="G29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F30" s="1">
+        <f>SUM(F2:F29)</f>
+        <v>882.82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>